<commit_message>
data in csv labeled
</commit_message>
<xml_diff>
--- a/ar1.xlsx
+++ b/ar1.xlsx
@@ -378,13 +378,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.09698873066568559</v>
+        <v>0.1831944722881327</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1328174467423007</v>
+        <v>0.04429341463183867</v>
       </c>
       <c r="E2" t="n">
-        <v>0.584325562401926</v>
+        <v>0.2603791776828435</v>
       </c>
     </row>
     <row r="3">
@@ -399,13 +399,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9639988021070259</v>
+        <v>0.07354921245638879</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6204839790649345</v>
+        <v>0.1451621806139535</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7215334415853583</v>
+        <v>0.3378236949304282</v>
       </c>
     </row>
     <row r="4">
@@ -420,13 +420,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9142731260480235</v>
+        <v>0.5140503535480559</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2221572838649597</v>
+        <v>0.7738762166124983</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7551033635468183</v>
+        <v>0.1778277411902804</v>
       </c>
     </row>
     <row r="5">
@@ -441,13 +441,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.118765898949006</v>
+        <v>0.04812471609263469</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2558484463390833</v>
+        <v>0.4372860710202552</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9936126184970845</v>
+        <v>0.0266144070951404</v>
       </c>
     </row>
     <row r="6">
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.02518329049972723</v>
+        <v>0.1622413097994405</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5081468377363142</v>
+        <v>0.8164297880401218</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3574920183825036</v>
+        <v>0.2471189745357338</v>
       </c>
     </row>
     <row r="7">
@@ -483,13 +483,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4446340570501159</v>
+        <v>0.1154468374321959</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3357471980792093</v>
+        <v>0.3985122619810699</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1309681293648562</v>
+        <v>0.1252276747800244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>